<commit_message>
fix: resolve job is not defined error when clearing selected job
</commit_message>
<xml_diff>
--- a/frontend/public/static/QuestionBank_Upload_Format.xlsx
+++ b/frontend/public/static/QuestionBank_Upload_Format.xlsx
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>